<commit_message>
faire version avec mission type
</commit_message>
<xml_diff>
--- a/data/visiteurs-aresia.xlsx
+++ b/data/visiteurs-aresia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Desktop\visiteurs-aresia-2025-06-04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Desktop\STAGE\excelpdf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C32875F-D63A-4214-A4B1-A0CC4671547F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C00B49D-783C-4AA9-A7D8-A785E82BFB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>./photos/ARESIA-M9TYSOMG-5EIM.jpg</t>
+  </si>
+  <si>
+    <t>Type de mission</t>
+  </si>
+  <si>
+    <t>AIR - GROUND</t>
+  </si>
+  <si>
+    <t>AIR - AIR</t>
   </si>
 </sst>
 </file>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -468,9 +477,10 @@
     <col min="2" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,8 +496,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -503,8 +516,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -520,8 +536,11 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -536,6 +555,9 @@
       </c>
       <c r="E4" t="s">
         <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>